<commit_message>
Update to 'AutoSPInstaller_Issue_Tracker' for Version 3.86
</commit_message>
<xml_diff>
--- a/SharePoint/AutoSPInstaller/AutoSPInstaller_Issue_Tracker.xlsx
+++ b/SharePoint/AutoSPInstaller/AutoSPInstaller_Issue_Tracker.xlsx
@@ -24,23 +24,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Issue</t>
   </si>
   <si>
-    <t>In the 'AutoSPInstallerInput'  XML file under the 'EnterpriseSearchService' section leave the default location for the search index in place: IndexLocation="C:\Program Files\Microsoft Office Servers\15.0\Data\Office Server\Applications"</t>
-  </si>
-  <si>
     <t>SharePoint Version</t>
   </si>
   <si>
     <t>AutoSPInstaller Version</t>
   </si>
   <si>
-    <t>When you specify a 'non default' search index location path in your 'IndexLocation' parameter in the 'AutoSPinstallerInput' XML file you get the following crawl log error: "The filtering process has been terminated"</t>
-  </si>
-  <si>
     <t>ChangeSet</t>
   </si>
   <si>
@@ -50,13 +44,25 @@
     <t>Solution</t>
   </si>
   <si>
-    <t>Meant to have been resolved in changeset 99077</t>
-  </si>
-  <si>
-    <t>When you launch the User Profile Service Application and attempt to edit your 'Synchronization Connections' created during the install; you get a 'Unable to process Put message' exception when attempting to save the changes</t>
-  </si>
-  <si>
-    <t>Creating a whole new Synchronization Connection in the User Profile Service Application under 'Synchronization' --&gt; 'Configure Synchronization Connections' should resolve this. Check and test this with the Forefront Synchronization Service Manager (FIM 2010) client that gets installed with SharePoint. This is the default location for the FIM client: C:\Program Files\Microsoft Office Servers\15.0\Synchronization Service\UIShell\miisclient.exe</t>
+    <t>When you specify a 'non default' search index location path in your 'IndexLocation' parameter in the 'AutoSPinstallerInput' XML file you get the following crawl log error: "The filtering process has been terminated".</t>
+  </si>
+  <si>
+    <t>When you launch the User Profile Service Application and attempt to edit your 'Synchronization Connections' created during the install; you get a 'Unable to process Put message' exception when attempting to save the changes.</t>
+  </si>
+  <si>
+    <t>When you run the 'AutoSPInstallerLaunch' BAT file during the 'PrerequisiteInstallerFiles' phase you get .Net 3.5.1 framework installation exception messages. Even when you change the '&lt;OfflineInstall&gt;true&lt;/OfflineInstall&gt;' value to 'false' in in the 'AutoSPinstallerInput' XML file; you still encounter issues with installing the framework.</t>
+  </si>
+  <si>
+    <t>In the 'AutoSPInstallerInput'  XML file under the 'EnterpriseSearchService' section leave the default location for the search index in place: IndexLocation="C:\Program Files\Microsoft Office Servers\15.0\Data\Office Server\Applications".</t>
+  </si>
+  <si>
+    <t>Creating a whole new Synchronization Connection in the User Profile Service Application under 'Synchronization' --&gt; 'Configure Synchronization Connections' should resolve this. Check and test this with the Forefront Synchronization Service Manager (FIM 2010) client that gets installed with SharePoint. This is the default location for the FIM client: C:\Program Files\Microsoft Office Servers\15.0\Synchronization Service\UIShell\miisclient.exe.</t>
+  </si>
+  <si>
+    <t>Meant to have been resolved in changeset 99077.</t>
+  </si>
+  <si>
+    <t>Copy all of the files from your Windows Server 2012 Installation media '\sources\sxs' location to your AutoSPInstaller  sxs directory '\SP\2013\SharePoint\PrerequisiteInstallerFiles\sxs'. Try running the AutoSPInstallerLaunch' BAT file again.</t>
   </si>
 </sst>
 </file>
@@ -92,16 +98,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -386,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -404,22 +407,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="150" x14ac:dyDescent="0.25">
@@ -433,13 +436,13 @@
         <v>95247</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="240" x14ac:dyDescent="0.25">
@@ -453,10 +456,27 @@
         <v>95247</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3.86</v>
+      </c>
+      <c r="C4" s="2">
+        <v>99664</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates To 'AutoSPInstaller' Solution Notes
</commit_message>
<xml_diff>
--- a/SharePoint/AutoSPInstaller/AutoSPInstaller_Issue_Tracker.xlsx
+++ b/SharePoint/AutoSPInstaller/AutoSPInstaller_Issue_Tracker.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Issue</t>
   </si>
@@ -72,16 +72,38 @@
   </si>
   <si>
     <t>In order for the script to complete and for the other service applications to be provisioned; the flag needs to be set to 'false' for the Managed Metadata Service application in the 'AutoSPInstallerInput' XML file. Re-run the script to complete provisioning the other service applications and then once everything else has been completed and provisioned you can: delete the original Managed Metadata Service application; change the flag back to 'true' in the 'AutoSPInstallerInput' XML file; and then run the 'AutoSPInstallerLaunch' BAT file again. This should then provision the Managed Metadata Service application, along with the proxy application.</t>
+  </si>
+  <si>
+    <t>Adding your Web Front End servers to the Query Component of the '&lt;EnterpriseSearchServiceApplications&gt;' section of the 'AutoSPInstallerInput' XML file should provide a work around for this. Another approach is to also add your Web Front End servers to the '&lt;ServiceApps&gt;' configuration section of the  'AutoSPInstallerInput' XML file. Important: If you have a 'Provision="true"' value for your particular Service Apps; this will not pick up the Web Front ends. You will need to provision these manually like the example below. '&lt;UserProfileServiceApp Provision="YourServerName1 YourServerName2 YourServerName3 YourServerName4"'</t>
+  </si>
+  <si>
+    <t>Resources</t>
+  </si>
+  <si>
+    <t>When you have a multi-server farm with dedicated Web Front End servers without any Search / Application Services running on them; the 'AutoSPInstallerInput' XML file doesn't have reference to them and when running the 'AutoSPInstallerLaunch' BAT file a message like the one below is encountered. '- There are other servers specified as farm members in:
+ - AutoSPInstallerInput.xml
+ - but &lt;RemoteInstall&gt; is not set to "true" - nothing else to do.'. The farm configuration appears unable to see the Web Front End servers and thinks they don't exist.</t>
+  </si>
+  <si>
+    <t>http://autospinstaller.codeplex.com/discussions/390039</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,10 +126,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -118,8 +141,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -398,10 +425,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,9 +440,10 @@
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
     <col min="5" max="5" width="30.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="45" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -433,8 +462,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>2013</v>
       </c>
@@ -454,7 +486,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2013</v>
       </c>
@@ -471,7 +503,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2013</v>
       </c>
@@ -488,7 +520,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="390" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="390" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2013</v>
       </c>
@@ -504,8 +536,9 @@
       <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="330" x14ac:dyDescent="0.25">
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="330" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2013</v>
       </c>
@@ -522,8 +555,31 @@
         <v>15</v>
       </c>
     </row>
+    <row r="7" spans="1:7" ht="345" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3.86</v>
+      </c>
+      <c r="C7" s="2">
+        <v>99664</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G7" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to 'AutoSPInstaller' Notes and Added SP2013 Calendar Overlays
</commit_message>
<xml_diff>
--- a/SharePoint/AutoSPInstaller/AutoSPInstaller_Issue_Tracker.xlsx
+++ b/SharePoint/AutoSPInstaller/AutoSPInstaller_Issue_Tracker.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Issue</t>
   </si>
@@ -86,6 +86,15 @@
   </si>
   <si>
     <t>http://autospinstaller.codeplex.com/discussions/390039</t>
+  </si>
+  <si>
+    <t>Tested with AutoSPInstaller Version 3.87, and issue appears to no longer occur.</t>
+  </si>
+  <si>
+    <t>Ensure that your SQL Server instance has mixed mode authentication enabled for both Windows and SQL logins. Properties --&gt; Security --&gt; SQL Server and Windows Authentication mode.</t>
+  </si>
+  <si>
+    <t>When you select 'True' to provision Access Services 2013 under your Enterprise Service Applications; and then encounter an exception message like the one below when you run the 'AutoSPInstallerLaunch' BAT file. 'New-SPAccessServicesApplication : A connection could be established to the Application Database Server but mixed mode authentication isn't enabled.'</t>
   </si>
 </sst>
 </file>
@@ -425,11 +434,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,8 +560,11 @@
       <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>15</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="345" x14ac:dyDescent="0.25">
@@ -573,6 +585,20 @@
       </c>
       <c r="G7" s="4" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3.87</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>